<commit_message>
Fix bug of vocabulary
</commit_message>
<xml_diff>
--- a/deploy-sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
+++ b/deploy-sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
@@ -942,9 +942,6 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Deploy Sakai and MySQL on a some server.</t>
-  </si>
-  <si>
     <t>User can explore directy the Sakai from the Tomcat URL http://&lt;server&gt;:8080/portal</t>
   </si>
   <si>
@@ -980,6 +977,9 @@
   </si>
   <si>
     <t>This text provide you some common mysql scripts or configurations for Sakai.</t>
+  </si>
+  <si>
+    <t>Deploy Sakai and MySQL on a same server.</t>
   </si>
 </sst>
 </file>
@@ -1314,6 +1314,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1350,38 +1369,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1702,10 +1702,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="76"/>
+      <c r="B3" s="60"/>
     </row>
     <row r="4" spans="1:3" ht="13.5" thickTop="1">
       <c r="B4" t="s">
@@ -1713,19 +1713,19 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="61" t="s">
         <v>291</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="60"/>
     </row>
     <row r="7" spans="1:3" ht="13.5" thickTop="1">
       <c r="B7" s="3" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1762,7 +1762,7 @@
       </c>
     </row>
     <row r="18" spans="3:3">
-      <c r="C18" s="78"/>
+      <c r="C18" s="62"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1794,7 +1794,7 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1812,12 +1812,12 @@
     </row>
     <row r="5" spans="1:17">
       <c r="B5" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="B6" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2317,7 +2317,7 @@
       <c r="C59" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D59" s="71" t="s">
+      <c r="D59" s="55" t="s">
         <v>253</v>
       </c>
       <c r="E59" s="5"/>
@@ -2858,36 +2858,36 @@
       <c r="V90" s="11"/>
     </row>
     <row r="91" spans="3:30" ht="60" customHeight="1">
-      <c r="C91" s="50" t="s">
+      <c r="C91" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="D91" s="50"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
-      <c r="G91" s="50"/>
-      <c r="H91" s="50"/>
-      <c r="I91" s="50"/>
-      <c r="J91" s="50"/>
-      <c r="K91" s="50"/>
-      <c r="L91" s="50"/>
-      <c r="M91" s="50"/>
-      <c r="N91" s="50"/>
-      <c r="O91" s="50"/>
-      <c r="P91" s="50"/>
-      <c r="Q91" s="50"/>
-      <c r="R91" s="50"/>
-      <c r="S91" s="50"/>
-      <c r="T91" s="50"/>
-      <c r="U91" s="50"/>
-      <c r="V91" s="50"/>
-      <c r="W91" s="50"/>
-      <c r="X91" s="50"/>
-      <c r="Y91" s="50"/>
-      <c r="Z91" s="50"/>
-      <c r="AA91" s="50"/>
-      <c r="AB91" s="50"/>
-      <c r="AC91" s="50"/>
-      <c r="AD91" s="50"/>
+      <c r="D91" s="63"/>
+      <c r="E91" s="63"/>
+      <c r="F91" s="63"/>
+      <c r="G91" s="63"/>
+      <c r="H91" s="63"/>
+      <c r="I91" s="63"/>
+      <c r="J91" s="63"/>
+      <c r="K91" s="63"/>
+      <c r="L91" s="63"/>
+      <c r="M91" s="63"/>
+      <c r="N91" s="63"/>
+      <c r="O91" s="63"/>
+      <c r="P91" s="63"/>
+      <c r="Q91" s="63"/>
+      <c r="R91" s="63"/>
+      <c r="S91" s="63"/>
+      <c r="T91" s="63"/>
+      <c r="U91" s="63"/>
+      <c r="V91" s="63"/>
+      <c r="W91" s="63"/>
+      <c r="X91" s="63"/>
+      <c r="Y91" s="63"/>
+      <c r="Z91" s="63"/>
+      <c r="AA91" s="63"/>
+      <c r="AB91" s="63"/>
+      <c r="AC91" s="63"/>
+      <c r="AD91" s="63"/>
     </row>
     <row r="92" spans="3:30">
       <c r="C92" s="31" t="s">
@@ -3658,186 +3658,186 @@
       <c r="V123" s="11"/>
     </row>
     <row r="124" spans="3:30">
-      <c r="C124" s="51" t="s">
+      <c r="C124" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="D124" s="52"/>
-      <c r="E124" s="52"/>
-      <c r="F124" s="52"/>
-      <c r="G124" s="52"/>
-      <c r="H124" s="52"/>
-      <c r="I124" s="52"/>
-      <c r="J124" s="52"/>
-      <c r="K124" s="52"/>
-      <c r="L124" s="52"/>
-      <c r="M124" s="52"/>
-      <c r="N124" s="52"/>
-      <c r="O124" s="52"/>
-      <c r="P124" s="52"/>
-      <c r="Q124" s="52"/>
-      <c r="R124" s="52"/>
-      <c r="S124" s="52"/>
-      <c r="T124" s="52"/>
-      <c r="U124" s="52"/>
-      <c r="V124" s="52"/>
-      <c r="W124" s="52"/>
-      <c r="X124" s="52"/>
-      <c r="Y124" s="52"/>
-      <c r="Z124" s="52"/>
-      <c r="AA124" s="52"/>
-      <c r="AB124" s="52"/>
-      <c r="AC124" s="52"/>
-      <c r="AD124" s="53"/>
+      <c r="D124" s="65"/>
+      <c r="E124" s="65"/>
+      <c r="F124" s="65"/>
+      <c r="G124" s="65"/>
+      <c r="H124" s="65"/>
+      <c r="I124" s="65"/>
+      <c r="J124" s="65"/>
+      <c r="K124" s="65"/>
+      <c r="L124" s="65"/>
+      <c r="M124" s="65"/>
+      <c r="N124" s="65"/>
+      <c r="O124" s="65"/>
+      <c r="P124" s="65"/>
+      <c r="Q124" s="65"/>
+      <c r="R124" s="65"/>
+      <c r="S124" s="65"/>
+      <c r="T124" s="65"/>
+      <c r="U124" s="65"/>
+      <c r="V124" s="65"/>
+      <c r="W124" s="65"/>
+      <c r="X124" s="65"/>
+      <c r="Y124" s="65"/>
+      <c r="Z124" s="65"/>
+      <c r="AA124" s="65"/>
+      <c r="AB124" s="65"/>
+      <c r="AC124" s="65"/>
+      <c r="AD124" s="66"/>
     </row>
     <row r="125" spans="3:30" ht="12.75" customHeight="1">
-      <c r="C125" s="54"/>
-      <c r="D125" s="50"/>
-      <c r="E125" s="50"/>
-      <c r="F125" s="50"/>
-      <c r="G125" s="50"/>
-      <c r="H125" s="50"/>
-      <c r="I125" s="50"/>
-      <c r="J125" s="50"/>
-      <c r="K125" s="50"/>
-      <c r="L125" s="50"/>
-      <c r="M125" s="50"/>
-      <c r="N125" s="50"/>
-      <c r="O125" s="50"/>
-      <c r="P125" s="50"/>
-      <c r="Q125" s="50"/>
-      <c r="R125" s="50"/>
-      <c r="S125" s="50"/>
-      <c r="T125" s="50"/>
-      <c r="U125" s="50"/>
-      <c r="V125" s="50"/>
-      <c r="W125" s="50"/>
-      <c r="X125" s="50"/>
-      <c r="Y125" s="50"/>
-      <c r="Z125" s="50"/>
-      <c r="AA125" s="50"/>
-      <c r="AB125" s="50"/>
-      <c r="AC125" s="50"/>
-      <c r="AD125" s="55"/>
+      <c r="C125" s="67"/>
+      <c r="D125" s="63"/>
+      <c r="E125" s="63"/>
+      <c r="F125" s="63"/>
+      <c r="G125" s="63"/>
+      <c r="H125" s="63"/>
+      <c r="I125" s="63"/>
+      <c r="J125" s="63"/>
+      <c r="K125" s="63"/>
+      <c r="L125" s="63"/>
+      <c r="M125" s="63"/>
+      <c r="N125" s="63"/>
+      <c r="O125" s="63"/>
+      <c r="P125" s="63"/>
+      <c r="Q125" s="63"/>
+      <c r="R125" s="63"/>
+      <c r="S125" s="63"/>
+      <c r="T125" s="63"/>
+      <c r="U125" s="63"/>
+      <c r="V125" s="63"/>
+      <c r="W125" s="63"/>
+      <c r="X125" s="63"/>
+      <c r="Y125" s="63"/>
+      <c r="Z125" s="63"/>
+      <c r="AA125" s="63"/>
+      <c r="AB125" s="63"/>
+      <c r="AC125" s="63"/>
+      <c r="AD125" s="68"/>
     </row>
     <row r="126" spans="3:30">
-      <c r="C126" s="54"/>
-      <c r="D126" s="50"/>
-      <c r="E126" s="50"/>
-      <c r="F126" s="50"/>
-      <c r="G126" s="50"/>
-      <c r="H126" s="50"/>
-      <c r="I126" s="50"/>
-      <c r="J126" s="50"/>
-      <c r="K126" s="50"/>
-      <c r="L126" s="50"/>
-      <c r="M126" s="50"/>
-      <c r="N126" s="50"/>
-      <c r="O126" s="50"/>
-      <c r="P126" s="50"/>
-      <c r="Q126" s="50"/>
-      <c r="R126" s="50"/>
-      <c r="S126" s="50"/>
-      <c r="T126" s="50"/>
-      <c r="U126" s="50"/>
-      <c r="V126" s="50"/>
-      <c r="W126" s="50"/>
-      <c r="X126" s="50"/>
-      <c r="Y126" s="50"/>
-      <c r="Z126" s="50"/>
-      <c r="AA126" s="50"/>
-      <c r="AB126" s="50"/>
-      <c r="AC126" s="50"/>
-      <c r="AD126" s="55"/>
+      <c r="C126" s="67"/>
+      <c r="D126" s="63"/>
+      <c r="E126" s="63"/>
+      <c r="F126" s="63"/>
+      <c r="G126" s="63"/>
+      <c r="H126" s="63"/>
+      <c r="I126" s="63"/>
+      <c r="J126" s="63"/>
+      <c r="K126" s="63"/>
+      <c r="L126" s="63"/>
+      <c r="M126" s="63"/>
+      <c r="N126" s="63"/>
+      <c r="O126" s="63"/>
+      <c r="P126" s="63"/>
+      <c r="Q126" s="63"/>
+      <c r="R126" s="63"/>
+      <c r="S126" s="63"/>
+      <c r="T126" s="63"/>
+      <c r="U126" s="63"/>
+      <c r="V126" s="63"/>
+      <c r="W126" s="63"/>
+      <c r="X126" s="63"/>
+      <c r="Y126" s="63"/>
+      <c r="Z126" s="63"/>
+      <c r="AA126" s="63"/>
+      <c r="AB126" s="63"/>
+      <c r="AC126" s="63"/>
+      <c r="AD126" s="68"/>
     </row>
     <row r="127" spans="3:30">
-      <c r="C127" s="54"/>
-      <c r="D127" s="50"/>
-      <c r="E127" s="50"/>
-      <c r="F127" s="50"/>
-      <c r="G127" s="50"/>
-      <c r="H127" s="50"/>
-      <c r="I127" s="50"/>
-      <c r="J127" s="50"/>
-      <c r="K127" s="50"/>
-      <c r="L127" s="50"/>
-      <c r="M127" s="50"/>
-      <c r="N127" s="50"/>
-      <c r="O127" s="50"/>
-      <c r="P127" s="50"/>
-      <c r="Q127" s="50"/>
-      <c r="R127" s="50"/>
-      <c r="S127" s="50"/>
-      <c r="T127" s="50"/>
-      <c r="U127" s="50"/>
-      <c r="V127" s="50"/>
-      <c r="W127" s="50"/>
-      <c r="X127" s="50"/>
-      <c r="Y127" s="50"/>
-      <c r="Z127" s="50"/>
-      <c r="AA127" s="50"/>
-      <c r="AB127" s="50"/>
-      <c r="AC127" s="50"/>
-      <c r="AD127" s="55"/>
+      <c r="C127" s="67"/>
+      <c r="D127" s="63"/>
+      <c r="E127" s="63"/>
+      <c r="F127" s="63"/>
+      <c r="G127" s="63"/>
+      <c r="H127" s="63"/>
+      <c r="I127" s="63"/>
+      <c r="J127" s="63"/>
+      <c r="K127" s="63"/>
+      <c r="L127" s="63"/>
+      <c r="M127" s="63"/>
+      <c r="N127" s="63"/>
+      <c r="O127" s="63"/>
+      <c r="P127" s="63"/>
+      <c r="Q127" s="63"/>
+      <c r="R127" s="63"/>
+      <c r="S127" s="63"/>
+      <c r="T127" s="63"/>
+      <c r="U127" s="63"/>
+      <c r="V127" s="63"/>
+      <c r="W127" s="63"/>
+      <c r="X127" s="63"/>
+      <c r="Y127" s="63"/>
+      <c r="Z127" s="63"/>
+      <c r="AA127" s="63"/>
+      <c r="AB127" s="63"/>
+      <c r="AC127" s="63"/>
+      <c r="AD127" s="68"/>
     </row>
     <row r="128" spans="3:30">
-      <c r="C128" s="54"/>
-      <c r="D128" s="50"/>
-      <c r="E128" s="50"/>
-      <c r="F128" s="50"/>
-      <c r="G128" s="50"/>
-      <c r="H128" s="50"/>
-      <c r="I128" s="50"/>
-      <c r="J128" s="50"/>
-      <c r="K128" s="50"/>
-      <c r="L128" s="50"/>
-      <c r="M128" s="50"/>
-      <c r="N128" s="50"/>
-      <c r="O128" s="50"/>
-      <c r="P128" s="50"/>
-      <c r="Q128" s="50"/>
-      <c r="R128" s="50"/>
-      <c r="S128" s="50"/>
-      <c r="T128" s="50"/>
-      <c r="U128" s="50"/>
-      <c r="V128" s="50"/>
-      <c r="W128" s="50"/>
-      <c r="X128" s="50"/>
-      <c r="Y128" s="50"/>
-      <c r="Z128" s="50"/>
-      <c r="AA128" s="50"/>
-      <c r="AB128" s="50"/>
-      <c r="AC128" s="50"/>
-      <c r="AD128" s="55"/>
+      <c r="C128" s="67"/>
+      <c r="D128" s="63"/>
+      <c r="E128" s="63"/>
+      <c r="F128" s="63"/>
+      <c r="G128" s="63"/>
+      <c r="H128" s="63"/>
+      <c r="I128" s="63"/>
+      <c r="J128" s="63"/>
+      <c r="K128" s="63"/>
+      <c r="L128" s="63"/>
+      <c r="M128" s="63"/>
+      <c r="N128" s="63"/>
+      <c r="O128" s="63"/>
+      <c r="P128" s="63"/>
+      <c r="Q128" s="63"/>
+      <c r="R128" s="63"/>
+      <c r="S128" s="63"/>
+      <c r="T128" s="63"/>
+      <c r="U128" s="63"/>
+      <c r="V128" s="63"/>
+      <c r="W128" s="63"/>
+      <c r="X128" s="63"/>
+      <c r="Y128" s="63"/>
+      <c r="Z128" s="63"/>
+      <c r="AA128" s="63"/>
+      <c r="AB128" s="63"/>
+      <c r="AC128" s="63"/>
+      <c r="AD128" s="68"/>
     </row>
     <row r="129" spans="1:30">
-      <c r="C129" s="56"/>
-      <c r="D129" s="57"/>
-      <c r="E129" s="57"/>
-      <c r="F129" s="57"/>
-      <c r="G129" s="57"/>
-      <c r="H129" s="57"/>
-      <c r="I129" s="57"/>
-      <c r="J129" s="57"/>
-      <c r="K129" s="57"/>
-      <c r="L129" s="57"/>
-      <c r="M129" s="57"/>
-      <c r="N129" s="57"/>
-      <c r="O129" s="57"/>
-      <c r="P129" s="57"/>
-      <c r="Q129" s="57"/>
-      <c r="R129" s="57"/>
-      <c r="S129" s="57"/>
-      <c r="T129" s="57"/>
-      <c r="U129" s="57"/>
-      <c r="V129" s="57"/>
-      <c r="W129" s="57"/>
-      <c r="X129" s="57"/>
-      <c r="Y129" s="57"/>
-      <c r="Z129" s="57"/>
-      <c r="AA129" s="57"/>
-      <c r="AB129" s="57"/>
-      <c r="AC129" s="57"/>
-      <c r="AD129" s="58"/>
+      <c r="C129" s="69"/>
+      <c r="D129" s="70"/>
+      <c r="E129" s="70"/>
+      <c r="F129" s="70"/>
+      <c r="G129" s="70"/>
+      <c r="H129" s="70"/>
+      <c r="I129" s="70"/>
+      <c r="J129" s="70"/>
+      <c r="K129" s="70"/>
+      <c r="L129" s="70"/>
+      <c r="M129" s="70"/>
+      <c r="N129" s="70"/>
+      <c r="O129" s="70"/>
+      <c r="P129" s="70"/>
+      <c r="Q129" s="70"/>
+      <c r="R129" s="70"/>
+      <c r="S129" s="70"/>
+      <c r="T129" s="70"/>
+      <c r="U129" s="70"/>
+      <c r="V129" s="70"/>
+      <c r="W129" s="70"/>
+      <c r="X129" s="70"/>
+      <c r="Y129" s="70"/>
+      <c r="Z129" s="70"/>
+      <c r="AA129" s="70"/>
+      <c r="AB129" s="70"/>
+      <c r="AC129" s="70"/>
+      <c r="AD129" s="71"/>
     </row>
     <row r="130" spans="1:30">
       <c r="C130" s="29"/>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="133" spans="1:30">
       <c r="C133" s="29"/>
-      <c r="D133" s="70" t="s">
+      <c r="D133" s="54" t="s">
         <v>131</v>
       </c>
       <c r="E133" s="11"/>
@@ -4280,7 +4280,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4644,13 +4644,13 @@
       <c r="V37" s="6"/>
     </row>
     <row r="39" spans="1:22">
-      <c r="C39" s="62" t="s">
+      <c r="C39" s="50" t="s">
         <v>214</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="41" spans="1:22">
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="51" t="s">
         <v>217</v>
       </c>
       <c r="D41" s="32"/>
@@ -4758,37 +4758,37 @@
       <c r="V50" s="6"/>
     </row>
     <row r="52" spans="2:31" ht="44.25" customHeight="1">
-      <c r="C52" s="51" t="s">
+      <c r="C52" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-      <c r="K52" s="52"/>
-      <c r="L52" s="52"/>
-      <c r="M52" s="52"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="52"/>
-      <c r="Q52" s="52"/>
-      <c r="R52" s="52"/>
-      <c r="S52" s="52"/>
-      <c r="T52" s="52"/>
-      <c r="U52" s="52"/>
-      <c r="V52" s="52"/>
-      <c r="W52" s="52"/>
-      <c r="X52" s="52"/>
-      <c r="Y52" s="52"/>
-      <c r="Z52" s="52"/>
-      <c r="AA52" s="52"/>
-      <c r="AB52" s="52"/>
-      <c r="AC52" s="52"/>
-      <c r="AD52" s="52"/>
-      <c r="AE52" s="53"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="65"/>
+      <c r="J52" s="65"/>
+      <c r="K52" s="65"/>
+      <c r="L52" s="65"/>
+      <c r="M52" s="65"/>
+      <c r="N52" s="65"/>
+      <c r="O52" s="65"/>
+      <c r="P52" s="65"/>
+      <c r="Q52" s="65"/>
+      <c r="R52" s="65"/>
+      <c r="S52" s="65"/>
+      <c r="T52" s="65"/>
+      <c r="U52" s="65"/>
+      <c r="V52" s="65"/>
+      <c r="W52" s="65"/>
+      <c r="X52" s="65"/>
+      <c r="Y52" s="65"/>
+      <c r="Z52" s="65"/>
+      <c r="AA52" s="65"/>
+      <c r="AB52" s="65"/>
+      <c r="AC52" s="65"/>
+      <c r="AD52" s="65"/>
+      <c r="AE52" s="66"/>
     </row>
     <row r="53" spans="2:31">
       <c r="C53" s="10"/>
@@ -4822,7 +4822,7 @@
       <c r="AE53" s="12"/>
     </row>
     <row r="54" spans="2:31">
-      <c r="C54" s="67" t="s">
+      <c r="C54" s="53" t="s">
         <v>246</v>
       </c>
       <c r="D54" s="14"/>
@@ -4873,45 +4873,45 @@
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="2:31">
-      <c r="C59" s="62" t="s">
+      <c r="C59" s="50" t="s">
         <v>234</v>
       </c>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="2:31" ht="28.5" customHeight="1">
-      <c r="C60" s="64" t="s">
+      <c r="C60" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D60" s="60" t="s">
+      <c r="D60" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="E60" s="60"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="60"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="60"/>
-      <c r="J60" s="60"/>
-      <c r="K60" s="60"/>
-      <c r="L60" s="60"/>
-      <c r="M60" s="60"/>
-      <c r="N60" s="60"/>
-      <c r="O60" s="60"/>
-      <c r="P60" s="60"/>
-      <c r="Q60" s="60"/>
-      <c r="R60" s="60"/>
-      <c r="S60" s="60"/>
-      <c r="T60" s="60"/>
-      <c r="U60" s="60"/>
-      <c r="V60" s="60"/>
-      <c r="W60" s="60"/>
-      <c r="X60" s="60"/>
-      <c r="Y60" s="60"/>
-      <c r="Z60" s="60"/>
-      <c r="AA60" s="60"/>
-      <c r="AB60" s="60"/>
-      <c r="AC60" s="60"/>
-      <c r="AD60" s="60"/>
-      <c r="AE60" s="61"/>
+      <c r="E60" s="73"/>
+      <c r="F60" s="73"/>
+      <c r="G60" s="73"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="73"/>
+      <c r="M60" s="73"/>
+      <c r="N60" s="73"/>
+      <c r="O60" s="73"/>
+      <c r="P60" s="73"/>
+      <c r="Q60" s="73"/>
+      <c r="R60" s="73"/>
+      <c r="S60" s="73"/>
+      <c r="T60" s="73"/>
+      <c r="U60" s="73"/>
+      <c r="V60" s="73"/>
+      <c r="W60" s="73"/>
+      <c r="X60" s="73"/>
+      <c r="Y60" s="73"/>
+      <c r="Z60" s="73"/>
+      <c r="AA60" s="73"/>
+      <c r="AB60" s="73"/>
+      <c r="AC60" s="73"/>
+      <c r="AD60" s="73"/>
+      <c r="AE60" s="74"/>
     </row>
     <row r="62" spans="2:31">
       <c r="C62" s="3" t="s">
@@ -5131,7 +5131,7 @@
       <c r="V71" s="11"/>
     </row>
     <row r="72" spans="3:31">
-      <c r="C72" s="63" t="s">
+      <c r="C72" s="51" t="s">
         <v>223</v>
       </c>
       <c r="D72" s="32"/>
@@ -5296,37 +5296,37 @@
       <c r="AE76" s="12"/>
     </row>
     <row r="77" spans="3:31" ht="27" customHeight="1">
-      <c r="C77" s="66" t="s">
+      <c r="C77" s="75" t="s">
         <v>240</v>
       </c>
-      <c r="D77" s="66"/>
-      <c r="E77" s="66"/>
-      <c r="F77" s="66"/>
-      <c r="G77" s="66"/>
-      <c r="H77" s="66"/>
-      <c r="I77" s="66"/>
-      <c r="J77" s="66"/>
-      <c r="K77" s="66"/>
-      <c r="L77" s="66"/>
-      <c r="M77" s="66"/>
-      <c r="N77" s="66"/>
-      <c r="O77" s="66"/>
-      <c r="P77" s="66"/>
-      <c r="Q77" s="66"/>
-      <c r="R77" s="66"/>
-      <c r="S77" s="66"/>
-      <c r="T77" s="66"/>
-      <c r="U77" s="66"/>
-      <c r="V77" s="66"/>
-      <c r="W77" s="66"/>
-      <c r="X77" s="66"/>
-      <c r="Y77" s="66"/>
-      <c r="Z77" s="66"/>
-      <c r="AA77" s="66"/>
-      <c r="AB77" s="66"/>
-      <c r="AC77" s="66"/>
-      <c r="AD77" s="66"/>
-      <c r="AE77" s="66"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
+      <c r="I77" s="75"/>
+      <c r="J77" s="75"/>
+      <c r="K77" s="75"/>
+      <c r="L77" s="75"/>
+      <c r="M77" s="75"/>
+      <c r="N77" s="75"/>
+      <c r="O77" s="75"/>
+      <c r="P77" s="75"/>
+      <c r="Q77" s="75"/>
+      <c r="R77" s="75"/>
+      <c r="S77" s="75"/>
+      <c r="T77" s="75"/>
+      <c r="U77" s="75"/>
+      <c r="V77" s="75"/>
+      <c r="W77" s="75"/>
+      <c r="X77" s="75"/>
+      <c r="Y77" s="75"/>
+      <c r="Z77" s="75"/>
+      <c r="AA77" s="75"/>
+      <c r="AB77" s="75"/>
+      <c r="AC77" s="75"/>
+      <c r="AD77" s="75"/>
+      <c r="AE77" s="75"/>
     </row>
     <row r="78" spans="3:31">
       <c r="C78" t="s">
@@ -5553,13 +5553,13 @@
       <c r="V85" s="11"/>
     </row>
     <row r="86" spans="2:31">
-      <c r="C86" s="72" t="s">
+      <c r="C86" s="56" t="s">
         <v>256</v>
       </c>
-      <c r="D86" s="72"/>
-      <c r="E86" s="73"/>
-      <c r="F86" s="73"/>
-      <c r="G86" s="73"/>
+      <c r="D86" s="56"/>
+      <c r="E86" s="57"/>
+      <c r="F86" s="57"/>
+      <c r="G86" s="57"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
@@ -5602,36 +5602,36 @@
     </row>
     <row r="88" spans="2:31" ht="27.75" customHeight="1">
       <c r="C88" s="29"/>
-      <c r="D88" s="59" t="s">
+      <c r="D88" s="72" t="s">
         <v>273</v>
       </c>
-      <c r="E88" s="60"/>
-      <c r="F88" s="60"/>
-      <c r="G88" s="60"/>
-      <c r="H88" s="60"/>
-      <c r="I88" s="60"/>
-      <c r="J88" s="60"/>
-      <c r="K88" s="60"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="60"/>
-      <c r="N88" s="60"/>
-      <c r="O88" s="60"/>
-      <c r="P88" s="60"/>
-      <c r="Q88" s="60"/>
-      <c r="R88" s="60"/>
-      <c r="S88" s="60"/>
-      <c r="T88" s="60"/>
-      <c r="U88" s="60"/>
-      <c r="V88" s="60"/>
-      <c r="W88" s="60"/>
-      <c r="X88" s="60"/>
-      <c r="Y88" s="60"/>
-      <c r="Z88" s="60"/>
-      <c r="AA88" s="60"/>
-      <c r="AB88" s="60"/>
-      <c r="AC88" s="60"/>
-      <c r="AD88" s="60"/>
-      <c r="AE88" s="61"/>
+      <c r="E88" s="73"/>
+      <c r="F88" s="73"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+      <c r="K88" s="73"/>
+      <c r="L88" s="73"/>
+      <c r="M88" s="73"/>
+      <c r="N88" s="73"/>
+      <c r="O88" s="73"/>
+      <c r="P88" s="73"/>
+      <c r="Q88" s="73"/>
+      <c r="R88" s="73"/>
+      <c r="S88" s="73"/>
+      <c r="T88" s="73"/>
+      <c r="U88" s="73"/>
+      <c r="V88" s="73"/>
+      <c r="W88" s="73"/>
+      <c r="X88" s="73"/>
+      <c r="Y88" s="73"/>
+      <c r="Z88" s="73"/>
+      <c r="AA88" s="73"/>
+      <c r="AB88" s="73"/>
+      <c r="AC88" s="73"/>
+      <c r="AD88" s="73"/>
+      <c r="AE88" s="74"/>
     </row>
     <row r="89" spans="2:31">
       <c r="C89" s="29"/>
@@ -5680,7 +5680,7 @@
       <c r="V90" s="11"/>
     </row>
     <row r="91" spans="2:31">
-      <c r="C91" s="74" t="s">
+      <c r="C91" s="58" t="s">
         <v>276</v>
       </c>
       <c r="D91" s="30"/>
@@ -6782,32 +6782,32 @@
     </row>
     <row r="8" spans="2:26" ht="41.25" customHeight="1">
       <c r="B8" s="10"/>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="76" t="s">
         <v>250</v>
       </c>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="68"/>
-      <c r="V8" s="68"/>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="68"/>
-      <c r="Z8" s="69"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="76"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="76"/>
+      <c r="V8" s="76"/>
+      <c r="W8" s="76"/>
+      <c r="X8" s="76"/>
+      <c r="Y8" s="76"/>
+      <c r="Z8" s="77"/>
     </row>
     <row r="9" spans="2:26">
       <c r="B9" s="10"/>
@@ -10393,7 +10393,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="48" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -10515,29 +10515,29 @@
       </c>
     </row>
     <row r="30" spans="2:22" ht="33" customHeight="1">
-      <c r="B30" s="65" t="s">
+      <c r="B30" s="79" t="s">
         <v>269</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="65"/>
-      <c r="N30" s="65"/>
-      <c r="O30" s="65"/>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="65"/>
-      <c r="R30" s="65"/>
-      <c r="S30" s="65"/>
-      <c r="T30" s="65"/>
-      <c r="U30" s="65"/>
-      <c r="V30" s="65"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="79"/>
+      <c r="T30" s="79"/>
+      <c r="U30" s="79"/>
+      <c r="V30" s="79"/>
     </row>
     <row r="31" spans="2:22">
       <c r="B31" s="49" t="s">
@@ -10555,28 +10555,28 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="91.5" customHeight="1">
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="78" t="s">
         <v>280</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="79"/>
-      <c r="S35" s="79"/>
-      <c r="T35" s="79"/>
-      <c r="U35" s="79"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="78"/>
+      <c r="S35" s="78"/>
+      <c r="T35" s="78"/>
+      <c r="U35" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Fix bug of English. Add more guidelines: 3	Exercise01_CreateCourseSite	Guideline to Create a training course siite 4	Exercise02_CreateQuestionBank	Guideline to create question bank for the e-learning system
</commit_message>
<xml_diff>
--- a/deploy-sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
+++ b/deploy-sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="11340" windowHeight="8535" tabRatio="991" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="11340" windowHeight="8535" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="9" r:id="rId1"/>
@@ -14,6 +14,9 @@
     <sheet name="_setenv.sh" sheetId="40" r:id="rId5"/>
     <sheet name="_tomcat-service" sheetId="29" r:id="rId6"/>
     <sheet name="MySQL" sheetId="5" r:id="rId7"/>
+    <sheet name="Exercise01_CreateCourseSite" sheetId="50" r:id="rId8"/>
+    <sheet name="Exercise02_CreateQuestionBank" sheetId="52" r:id="rId9"/>
+    <sheet name="Template" sheetId="53" state="hidden" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Linux!$A$1:$AE$146</definedName>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="357">
   <si>
     <t>#</t>
   </si>
@@ -981,6 +984,199 @@
   <si>
     <t>Prerequisites:</t>
   </si>
+  <si>
+    <t>Login to the sakai</t>
+  </si>
+  <si>
+    <t>URL: http://&lt;your server ip&gt;: 8080/portal</t>
+  </si>
+  <si>
+    <t>Username: admin</t>
+  </si>
+  <si>
+    <t>Password: admin</t>
+  </si>
+  <si>
+    <t>Click on this help icon to learn the features on sakai.</t>
+  </si>
+  <si>
+    <t>Create a site for a course</t>
+  </si>
+  <si>
+    <t>Context:</t>
+  </si>
+  <si>
+    <t>We want to build a site for training, online testing</t>
+  </si>
+  <si>
+    <t>How to create?</t>
+  </si>
+  <si>
+    <t>Login with account admin. Then perform below steps:</t>
+  </si>
+  <si>
+    <t>Click on Worksite Setup in left menu</t>
+  </si>
+  <si>
+    <t>Then click on button "New" in the top screen of "My Workspace: Worksite Setup"</t>
+  </si>
+  <si>
+    <t>Select course site</t>
+  </si>
+  <si>
+    <t>Trouble shooting:</t>
+  </si>
+  <si>
+    <t>Default account:</t>
+  </si>
+  <si>
+    <t>If you don't see any item in Academic term, please check in sheet "Sakai", section</t>
+  </si>
+  <si>
+    <t>2.c) Create "Academic term"</t>
+  </si>
+  <si>
+    <t>Select course section</t>
+  </si>
+  <si>
+    <t>Input information for Course</t>
+  </si>
+  <si>
+    <t>Subject: input your course name</t>
+  </si>
+  <si>
+    <t>Course: input any code (we will changed it later)</t>
+  </si>
+  <si>
+    <t>Section: input any code (we will changed it later)</t>
+  </si>
+  <si>
+    <t>Authorizer's username: admin</t>
+  </si>
+  <si>
+    <t>Select Language, input Course Introduction</t>
+  </si>
+  <si>
+    <t>Select tools for course site</t>
+  </si>
+  <si>
+    <t>Please select more tools:</t>
+  </si>
+  <si>
+    <t>Then, click on button "Continue" twice. Finally, click on button "Request site".</t>
+  </si>
+  <si>
+    <t>Edit site</t>
+  </si>
+  <si>
+    <t>Click on left menu "Sites"</t>
+  </si>
+  <si>
+    <t>Search "MyCourse". Then click on link of Site Id</t>
+  </si>
+  <si>
+    <t>Search created site</t>
+  </si>
+  <si>
+    <t>Change Title, Site URL Alias</t>
+  </si>
+  <si>
+    <t>(Ex: My test server is 1088.16.135. So the link is "http://10.88.16.135:8080")</t>
+  </si>
+  <si>
+    <r>
+      <t>Click link "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Still cannot find your course/section?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Ex: Change Title to "Java Fresher"</t>
+  </si>
+  <si>
+    <t>Change Site URL Alias to "javafresher"</t>
+  </si>
+  <si>
+    <t>Then, click on button "Save".</t>
+  </si>
+  <si>
+    <t>Change setting the order of sites</t>
+  </si>
+  <si>
+    <t>Click on left menu "Preferences". Then drag the course "JavaFresher" from column "Active Sites" into the "My Workspace"</t>
+  </si>
+  <si>
+    <t>Then, click of button "Update Preferences".</t>
+  </si>
+  <si>
+    <t>Click any site "Administration Workspace" or "Ciations Admin", etc to refresh the bar of sites.</t>
+  </si>
+  <si>
+    <t>Create Question Bank</t>
+  </si>
+  <si>
+    <t>Click on the course site such as "JavaFresher".</t>
+  </si>
+  <si>
+    <t>Click on left menu "Tests &amp; Quizzes".</t>
+  </si>
+  <si>
+    <t>Create Question Pool</t>
+  </si>
+  <si>
+    <t>Click on link "Add New Pool"</t>
+  </si>
+  <si>
+    <t>Input information for Pool</t>
+  </si>
+  <si>
+    <t>Then click on button "Save"</t>
+  </si>
+  <si>
+    <t>Click on link of Pool Name</t>
+  </si>
+  <si>
+    <t>Create Question</t>
+  </si>
+  <si>
+    <t>Select question type.</t>
+  </si>
+  <si>
+    <t>Ex: Select Multiple Choice</t>
+  </si>
+  <si>
+    <t>Input information for question: Question Text, Options, select correct option; Randomize options or not.</t>
+  </si>
+  <si>
+    <t>Select "Yes" for section "Randomize Answers" if your optional answers have not item or similar item such as "Both A and B are true".</t>
+  </si>
+  <si>
+    <t>Exercise01_CreateCourseSite</t>
+  </si>
+  <si>
+    <t>Guideline to Create a training course siite</t>
+  </si>
+  <si>
+    <t>Guideline to create question bank for the e-learning system</t>
+  </si>
+  <si>
+    <t>Exercise02_CreateQuestionBank</t>
+  </si>
 </sst>
 </file>
 
@@ -990,7 +1186,7 @@
     <numFmt numFmtId="164" formatCode="#."/>
     <numFmt numFmtId="165" formatCode="#\)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1052,6 +1248,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1073,7 +1281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1233,6 +1441,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1241,7 +1469,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1333,6 +1561,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1398,6 +1638,2834 @@
     </mruColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>65705</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142233</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="219076" y="1162050"/>
+          <a:ext cx="7771429" cy="5142858"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Up Arrow 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7467600" y="3857625"/>
+          <a:ext cx="200025" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="upArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>119063</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7419975" y="4533900"/>
+          <a:ext cx="147638" cy="2076450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>8676</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>19402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1032" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="8429626"/>
+          <a:ext cx="6800000" cy="4820001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rounded Rectangle 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="9772650"/>
+          <a:ext cx="381000" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1033" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="20221575"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1034" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="26889075"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rounded Rectangle 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="504825" y="10772775"/>
+          <a:ext cx="1123950" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="18" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1114425" y="10048875"/>
+          <a:ext cx="638175" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="15878175"/>
+          <a:ext cx="1905000" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Rounded Rectangle 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1724025" y="16592550"/>
+          <a:ext cx="571500" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rounded Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1685924" y="24241125"/>
+          <a:ext cx="1752601" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1036" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="33766125"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rounded Rectangle 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1771649" y="29613224"/>
+          <a:ext cx="3305176" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rounded Rectangle 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3295649" y="31994474"/>
+          <a:ext cx="2609851" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rounded Rectangle 30"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1724025" y="33280349"/>
+          <a:ext cx="561976" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1037" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="33804225"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rounded Rectangle 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514724" y="35442524"/>
+          <a:ext cx="3048001" cy="828676"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Rounded Rectangle 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914524" y="37299899"/>
+          <a:ext cx="3048001" cy="828676"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rounded Rectangle 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1704974" y="38766749"/>
+          <a:ext cx="571501" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>8676</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>19402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1038" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="40490776"/>
+          <a:ext cx="6800000" cy="4820001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rounded Rectangle 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="43243499"/>
+          <a:ext cx="238126" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="657225" y="46205775"/>
+          <a:ext cx="2743200" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="657225" y="46396275"/>
+          <a:ext cx="2590800" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1046" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="47167800"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rounded Rectangle 45"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809624" y="50168174"/>
+          <a:ext cx="895351" cy="323851"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>301</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1047" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="53835300"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rounded Rectangle 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2352674" y="56387999"/>
+          <a:ext cx="990601" cy="314326"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Rounded Rectangle 48"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3409950" y="56387999"/>
+          <a:ext cx="485776" cy="314326"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>289</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rounded Rectangle 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1704974" y="57702449"/>
+          <a:ext cx="1400176" cy="314326"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>309</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1049" name="Picture 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="60721875"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>322</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rounded Rectangle 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3200399" y="64455674"/>
+          <a:ext cx="3152776" cy="542926"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>342</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="476251" y="68427600"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rounded Rectangle 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495299" y="73409174"/>
+          <a:ext cx="1228726" cy="428626"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>364</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>364</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Arrow Connector 39"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3543300" y="72847200"/>
+          <a:ext cx="1114425" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="800100"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rounded Rectangle 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="581025" y="3286125"/>
+          <a:ext cx="1057275" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rounded Rectangle 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3409950" y="2390775"/>
+          <a:ext cx="847725" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rounded Rectangle 42"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5448300" y="1371600"/>
+          <a:ext cx="990600" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Arrow Connector 44"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="40" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1109663" y="1581150"/>
+          <a:ext cx="4291012" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Arrow Connector 46"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="3"/>
+          <a:endCxn id="42" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1638300" y="2647950"/>
+          <a:ext cx="2195513" cy="766763"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="7200900"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rounded Rectangle 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1685925" y="9372600"/>
+          <a:ext cx="1057275" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2051" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="13801725"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rounded Rectangle 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1809750" y="17649825"/>
+          <a:ext cx="390525" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="20802600"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Rounded Rectangle 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2238375" y="23383875"/>
+          <a:ext cx="1285875" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2053" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="27603450"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Rounded Rectangle 55"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="32394525"/>
+          <a:ext cx="914400" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2054" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="34404300"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2055" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="41205150"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2056" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="48006000"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Rounded Rectangle 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1695450" y="36690300"/>
+          <a:ext cx="409575" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Rounded Rectangle 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2971800" y="35966400"/>
+          <a:ext cx="1609725" cy="2019300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Rounded Rectangle 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2000250" y="50320575"/>
+          <a:ext cx="1152525" cy="485776"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1687,12 +4755,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="A13:C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1761,6 +4831,28 @@
         <v>197</v>
       </c>
     </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="17">
+        <v>3</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="17">
+        <v>4</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>355</v>
+      </c>
+    </row>
     <row r="18" spans="3:3">
       <c r="C18" s="62"/>
     </row>
@@ -1769,12 +4861,33 @@
   <hyperlinks>
     <hyperlink ref="B11" location="Linux!A1" display="Linux"/>
     <hyperlink ref="B12" location="Sakai!A1" display="Sakai"/>
+    <hyperlink ref="B13" location="Exercise01_CreateCourseSite!A1" display="Exercise01_CreateCourseSite"/>
+    <hyperlink ref="B14" location="Exercise02_CreateQuestionBank!A1" display="Exercise02_CreateQuestionBank"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.4" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Symbol,Regular"Ó&amp;"Arial,Regular" Thach N. Le&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="7" width="3.28515625" style="47"/>
+    <col min="8" max="16384" width="3.28515625" style="63"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2858,36 +5971,36 @@
       <c r="V90" s="11"/>
     </row>
     <row r="91" spans="3:30" ht="60" customHeight="1">
-      <c r="C91" s="63" t="s">
+      <c r="C91" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="D91" s="63"/>
-      <c r="E91" s="63"/>
-      <c r="F91" s="63"/>
-      <c r="G91" s="63"/>
-      <c r="H91" s="63"/>
-      <c r="I91" s="63"/>
-      <c r="J91" s="63"/>
-      <c r="K91" s="63"/>
-      <c r="L91" s="63"/>
-      <c r="M91" s="63"/>
-      <c r="N91" s="63"/>
-      <c r="O91" s="63"/>
-      <c r="P91" s="63"/>
-      <c r="Q91" s="63"/>
-      <c r="R91" s="63"/>
-      <c r="S91" s="63"/>
-      <c r="T91" s="63"/>
-      <c r="U91" s="63"/>
-      <c r="V91" s="63"/>
-      <c r="W91" s="63"/>
-      <c r="X91" s="63"/>
-      <c r="Y91" s="63"/>
-      <c r="Z91" s="63"/>
-      <c r="AA91" s="63"/>
-      <c r="AB91" s="63"/>
-      <c r="AC91" s="63"/>
-      <c r="AD91" s="63"/>
+      <c r="D91" s="73"/>
+      <c r="E91" s="73"/>
+      <c r="F91" s="73"/>
+      <c r="G91" s="73"/>
+      <c r="H91" s="73"/>
+      <c r="I91" s="73"/>
+      <c r="J91" s="73"/>
+      <c r="K91" s="73"/>
+      <c r="L91" s="73"/>
+      <c r="M91" s="73"/>
+      <c r="N91" s="73"/>
+      <c r="O91" s="73"/>
+      <c r="P91" s="73"/>
+      <c r="Q91" s="73"/>
+      <c r="R91" s="73"/>
+      <c r="S91" s="73"/>
+      <c r="T91" s="73"/>
+      <c r="U91" s="73"/>
+      <c r="V91" s="73"/>
+      <c r="W91" s="73"/>
+      <c r="X91" s="73"/>
+      <c r="Y91" s="73"/>
+      <c r="Z91" s="73"/>
+      <c r="AA91" s="73"/>
+      <c r="AB91" s="73"/>
+      <c r="AC91" s="73"/>
+      <c r="AD91" s="73"/>
     </row>
     <row r="92" spans="3:30">
       <c r="C92" s="31" t="s">
@@ -3658,186 +6771,186 @@
       <c r="V123" s="11"/>
     </row>
     <row r="124" spans="3:30">
-      <c r="C124" s="64" t="s">
+      <c r="C124" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="D124" s="65"/>
-      <c r="E124" s="65"/>
-      <c r="F124" s="65"/>
-      <c r="G124" s="65"/>
-      <c r="H124" s="65"/>
-      <c r="I124" s="65"/>
-      <c r="J124" s="65"/>
-      <c r="K124" s="65"/>
-      <c r="L124" s="65"/>
-      <c r="M124" s="65"/>
-      <c r="N124" s="65"/>
-      <c r="O124" s="65"/>
-      <c r="P124" s="65"/>
-      <c r="Q124" s="65"/>
-      <c r="R124" s="65"/>
-      <c r="S124" s="65"/>
-      <c r="T124" s="65"/>
-      <c r="U124" s="65"/>
-      <c r="V124" s="65"/>
-      <c r="W124" s="65"/>
-      <c r="X124" s="65"/>
-      <c r="Y124" s="65"/>
-      <c r="Z124" s="65"/>
-      <c r="AA124" s="65"/>
-      <c r="AB124" s="65"/>
-      <c r="AC124" s="65"/>
-      <c r="AD124" s="66"/>
+      <c r="D124" s="75"/>
+      <c r="E124" s="75"/>
+      <c r="F124" s="75"/>
+      <c r="G124" s="75"/>
+      <c r="H124" s="75"/>
+      <c r="I124" s="75"/>
+      <c r="J124" s="75"/>
+      <c r="K124" s="75"/>
+      <c r="L124" s="75"/>
+      <c r="M124" s="75"/>
+      <c r="N124" s="75"/>
+      <c r="O124" s="75"/>
+      <c r="P124" s="75"/>
+      <c r="Q124" s="75"/>
+      <c r="R124" s="75"/>
+      <c r="S124" s="75"/>
+      <c r="T124" s="75"/>
+      <c r="U124" s="75"/>
+      <c r="V124" s="75"/>
+      <c r="W124" s="75"/>
+      <c r="X124" s="75"/>
+      <c r="Y124" s="75"/>
+      <c r="Z124" s="75"/>
+      <c r="AA124" s="75"/>
+      <c r="AB124" s="75"/>
+      <c r="AC124" s="75"/>
+      <c r="AD124" s="76"/>
     </row>
     <row r="125" spans="3:30" ht="12.75" customHeight="1">
-      <c r="C125" s="67"/>
-      <c r="D125" s="63"/>
-      <c r="E125" s="63"/>
-      <c r="F125" s="63"/>
-      <c r="G125" s="63"/>
-      <c r="H125" s="63"/>
-      <c r="I125" s="63"/>
-      <c r="J125" s="63"/>
-      <c r="K125" s="63"/>
-      <c r="L125" s="63"/>
-      <c r="M125" s="63"/>
-      <c r="N125" s="63"/>
-      <c r="O125" s="63"/>
-      <c r="P125" s="63"/>
-      <c r="Q125" s="63"/>
-      <c r="R125" s="63"/>
-      <c r="S125" s="63"/>
-      <c r="T125" s="63"/>
-      <c r="U125" s="63"/>
-      <c r="V125" s="63"/>
-      <c r="W125" s="63"/>
-      <c r="X125" s="63"/>
-      <c r="Y125" s="63"/>
-      <c r="Z125" s="63"/>
-      <c r="AA125" s="63"/>
-      <c r="AB125" s="63"/>
-      <c r="AC125" s="63"/>
-      <c r="AD125" s="68"/>
+      <c r="C125" s="77"/>
+      <c r="D125" s="73"/>
+      <c r="E125" s="73"/>
+      <c r="F125" s="73"/>
+      <c r="G125" s="73"/>
+      <c r="H125" s="73"/>
+      <c r="I125" s="73"/>
+      <c r="J125" s="73"/>
+      <c r="K125" s="73"/>
+      <c r="L125" s="73"/>
+      <c r="M125" s="73"/>
+      <c r="N125" s="73"/>
+      <c r="O125" s="73"/>
+      <c r="P125" s="73"/>
+      <c r="Q125" s="73"/>
+      <c r="R125" s="73"/>
+      <c r="S125" s="73"/>
+      <c r="T125" s="73"/>
+      <c r="U125" s="73"/>
+      <c r="V125" s="73"/>
+      <c r="W125" s="73"/>
+      <c r="X125" s="73"/>
+      <c r="Y125" s="73"/>
+      <c r="Z125" s="73"/>
+      <c r="AA125" s="73"/>
+      <c r="AB125" s="73"/>
+      <c r="AC125" s="73"/>
+      <c r="AD125" s="78"/>
     </row>
     <row r="126" spans="3:30">
-      <c r="C126" s="67"/>
-      <c r="D126" s="63"/>
-      <c r="E126" s="63"/>
-      <c r="F126" s="63"/>
-      <c r="G126" s="63"/>
-      <c r="H126" s="63"/>
-      <c r="I126" s="63"/>
-      <c r="J126" s="63"/>
-      <c r="K126" s="63"/>
-      <c r="L126" s="63"/>
-      <c r="M126" s="63"/>
-      <c r="N126" s="63"/>
-      <c r="O126" s="63"/>
-      <c r="P126" s="63"/>
-      <c r="Q126" s="63"/>
-      <c r="R126" s="63"/>
-      <c r="S126" s="63"/>
-      <c r="T126" s="63"/>
-      <c r="U126" s="63"/>
-      <c r="V126" s="63"/>
-      <c r="W126" s="63"/>
-      <c r="X126" s="63"/>
-      <c r="Y126" s="63"/>
-      <c r="Z126" s="63"/>
-      <c r="AA126" s="63"/>
-      <c r="AB126" s="63"/>
-      <c r="AC126" s="63"/>
-      <c r="AD126" s="68"/>
+      <c r="C126" s="77"/>
+      <c r="D126" s="73"/>
+      <c r="E126" s="73"/>
+      <c r="F126" s="73"/>
+      <c r="G126" s="73"/>
+      <c r="H126" s="73"/>
+      <c r="I126" s="73"/>
+      <c r="J126" s="73"/>
+      <c r="K126" s="73"/>
+      <c r="L126" s="73"/>
+      <c r="M126" s="73"/>
+      <c r="N126" s="73"/>
+      <c r="O126" s="73"/>
+      <c r="P126" s="73"/>
+      <c r="Q126" s="73"/>
+      <c r="R126" s="73"/>
+      <c r="S126" s="73"/>
+      <c r="T126" s="73"/>
+      <c r="U126" s="73"/>
+      <c r="V126" s="73"/>
+      <c r="W126" s="73"/>
+      <c r="X126" s="73"/>
+      <c r="Y126" s="73"/>
+      <c r="Z126" s="73"/>
+      <c r="AA126" s="73"/>
+      <c r="AB126" s="73"/>
+      <c r="AC126" s="73"/>
+      <c r="AD126" s="78"/>
     </row>
     <row r="127" spans="3:30">
-      <c r="C127" s="67"/>
-      <c r="D127" s="63"/>
-      <c r="E127" s="63"/>
-      <c r="F127" s="63"/>
-      <c r="G127" s="63"/>
-      <c r="H127" s="63"/>
-      <c r="I127" s="63"/>
-      <c r="J127" s="63"/>
-      <c r="K127" s="63"/>
-      <c r="L127" s="63"/>
-      <c r="M127" s="63"/>
-      <c r="N127" s="63"/>
-      <c r="O127" s="63"/>
-      <c r="P127" s="63"/>
-      <c r="Q127" s="63"/>
-      <c r="R127" s="63"/>
-      <c r="S127" s="63"/>
-      <c r="T127" s="63"/>
-      <c r="U127" s="63"/>
-      <c r="V127" s="63"/>
-      <c r="W127" s="63"/>
-      <c r="X127" s="63"/>
-      <c r="Y127" s="63"/>
-      <c r="Z127" s="63"/>
-      <c r="AA127" s="63"/>
-      <c r="AB127" s="63"/>
-      <c r="AC127" s="63"/>
-      <c r="AD127" s="68"/>
+      <c r="C127" s="77"/>
+      <c r="D127" s="73"/>
+      <c r="E127" s="73"/>
+      <c r="F127" s="73"/>
+      <c r="G127" s="73"/>
+      <c r="H127" s="73"/>
+      <c r="I127" s="73"/>
+      <c r="J127" s="73"/>
+      <c r="K127" s="73"/>
+      <c r="L127" s="73"/>
+      <c r="M127" s="73"/>
+      <c r="N127" s="73"/>
+      <c r="O127" s="73"/>
+      <c r="P127" s="73"/>
+      <c r="Q127" s="73"/>
+      <c r="R127" s="73"/>
+      <c r="S127" s="73"/>
+      <c r="T127" s="73"/>
+      <c r="U127" s="73"/>
+      <c r="V127" s="73"/>
+      <c r="W127" s="73"/>
+      <c r="X127" s="73"/>
+      <c r="Y127" s="73"/>
+      <c r="Z127" s="73"/>
+      <c r="AA127" s="73"/>
+      <c r="AB127" s="73"/>
+      <c r="AC127" s="73"/>
+      <c r="AD127" s="78"/>
     </row>
     <row r="128" spans="3:30">
-      <c r="C128" s="67"/>
-      <c r="D128" s="63"/>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
-      <c r="H128" s="63"/>
-      <c r="I128" s="63"/>
-      <c r="J128" s="63"/>
-      <c r="K128" s="63"/>
-      <c r="L128" s="63"/>
-      <c r="M128" s="63"/>
-      <c r="N128" s="63"/>
-      <c r="O128" s="63"/>
-      <c r="P128" s="63"/>
-      <c r="Q128" s="63"/>
-      <c r="R128" s="63"/>
-      <c r="S128" s="63"/>
-      <c r="T128" s="63"/>
-      <c r="U128" s="63"/>
-      <c r="V128" s="63"/>
-      <c r="W128" s="63"/>
-      <c r="X128" s="63"/>
-      <c r="Y128" s="63"/>
-      <c r="Z128" s="63"/>
-      <c r="AA128" s="63"/>
-      <c r="AB128" s="63"/>
-      <c r="AC128" s="63"/>
-      <c r="AD128" s="68"/>
+      <c r="C128" s="77"/>
+      <c r="D128" s="73"/>
+      <c r="E128" s="73"/>
+      <c r="F128" s="73"/>
+      <c r="G128" s="73"/>
+      <c r="H128" s="73"/>
+      <c r="I128" s="73"/>
+      <c r="J128" s="73"/>
+      <c r="K128" s="73"/>
+      <c r="L128" s="73"/>
+      <c r="M128" s="73"/>
+      <c r="N128" s="73"/>
+      <c r="O128" s="73"/>
+      <c r="P128" s="73"/>
+      <c r="Q128" s="73"/>
+      <c r="R128" s="73"/>
+      <c r="S128" s="73"/>
+      <c r="T128" s="73"/>
+      <c r="U128" s="73"/>
+      <c r="V128" s="73"/>
+      <c r="W128" s="73"/>
+      <c r="X128" s="73"/>
+      <c r="Y128" s="73"/>
+      <c r="Z128" s="73"/>
+      <c r="AA128" s="73"/>
+      <c r="AB128" s="73"/>
+      <c r="AC128" s="73"/>
+      <c r="AD128" s="78"/>
     </row>
     <row r="129" spans="1:30">
-      <c r="C129" s="69"/>
-      <c r="D129" s="70"/>
-      <c r="E129" s="70"/>
-      <c r="F129" s="70"/>
-      <c r="G129" s="70"/>
-      <c r="H129" s="70"/>
-      <c r="I129" s="70"/>
-      <c r="J129" s="70"/>
-      <c r="K129" s="70"/>
-      <c r="L129" s="70"/>
-      <c r="M129" s="70"/>
-      <c r="N129" s="70"/>
-      <c r="O129" s="70"/>
-      <c r="P129" s="70"/>
-      <c r="Q129" s="70"/>
-      <c r="R129" s="70"/>
-      <c r="S129" s="70"/>
-      <c r="T129" s="70"/>
-      <c r="U129" s="70"/>
-      <c r="V129" s="70"/>
-      <c r="W129" s="70"/>
-      <c r="X129" s="70"/>
-      <c r="Y129" s="70"/>
-      <c r="Z129" s="70"/>
-      <c r="AA129" s="70"/>
-      <c r="AB129" s="70"/>
-      <c r="AC129" s="70"/>
-      <c r="AD129" s="71"/>
+      <c r="C129" s="79"/>
+      <c r="D129" s="80"/>
+      <c r="E129" s="80"/>
+      <c r="F129" s="80"/>
+      <c r="G129" s="80"/>
+      <c r="H129" s="80"/>
+      <c r="I129" s="80"/>
+      <c r="J129" s="80"/>
+      <c r="K129" s="80"/>
+      <c r="L129" s="80"/>
+      <c r="M129" s="80"/>
+      <c r="N129" s="80"/>
+      <c r="O129" s="80"/>
+      <c r="P129" s="80"/>
+      <c r="Q129" s="80"/>
+      <c r="R129" s="80"/>
+      <c r="S129" s="80"/>
+      <c r="T129" s="80"/>
+      <c r="U129" s="80"/>
+      <c r="V129" s="80"/>
+      <c r="W129" s="80"/>
+      <c r="X129" s="80"/>
+      <c r="Y129" s="80"/>
+      <c r="Z129" s="80"/>
+      <c r="AA129" s="80"/>
+      <c r="AB129" s="80"/>
+      <c r="AC129" s="80"/>
+      <c r="AD129" s="81"/>
     </row>
     <row r="130" spans="1:30">
       <c r="C130" s="29"/>
@@ -4268,8 +7381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="12.75"/>
@@ -4758,37 +7871,37 @@
       <c r="V50" s="6"/>
     </row>
     <row r="52" spans="2:31" ht="44.25" customHeight="1">
-      <c r="C52" s="64" t="s">
+      <c r="C52" s="74" t="s">
         <v>243</v>
       </c>
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="65"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="65"/>
-      <c r="I52" s="65"/>
-      <c r="J52" s="65"/>
-      <c r="K52" s="65"/>
-      <c r="L52" s="65"/>
-      <c r="M52" s="65"/>
-      <c r="N52" s="65"/>
-      <c r="O52" s="65"/>
-      <c r="P52" s="65"/>
-      <c r="Q52" s="65"/>
-      <c r="R52" s="65"/>
-      <c r="S52" s="65"/>
-      <c r="T52" s="65"/>
-      <c r="U52" s="65"/>
-      <c r="V52" s="65"/>
-      <c r="W52" s="65"/>
-      <c r="X52" s="65"/>
-      <c r="Y52" s="65"/>
-      <c r="Z52" s="65"/>
-      <c r="AA52" s="65"/>
-      <c r="AB52" s="65"/>
-      <c r="AC52" s="65"/>
-      <c r="AD52" s="65"/>
-      <c r="AE52" s="66"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
+      <c r="L52" s="75"/>
+      <c r="M52" s="75"/>
+      <c r="N52" s="75"/>
+      <c r="O52" s="75"/>
+      <c r="P52" s="75"/>
+      <c r="Q52" s="75"/>
+      <c r="R52" s="75"/>
+      <c r="S52" s="75"/>
+      <c r="T52" s="75"/>
+      <c r="U52" s="75"/>
+      <c r="V52" s="75"/>
+      <c r="W52" s="75"/>
+      <c r="X52" s="75"/>
+      <c r="Y52" s="75"/>
+      <c r="Z52" s="75"/>
+      <c r="AA52" s="75"/>
+      <c r="AB52" s="75"/>
+      <c r="AC52" s="75"/>
+      <c r="AD52" s="75"/>
+      <c r="AE52" s="76"/>
     </row>
     <row r="53" spans="2:31">
       <c r="C53" s="10"/>
@@ -4882,36 +7995,36 @@
       <c r="C60" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D60" s="73" t="s">
+      <c r="D60" s="83" t="s">
         <v>218</v>
       </c>
-      <c r="E60" s="73"/>
-      <c r="F60" s="73"/>
-      <c r="G60" s="73"/>
-      <c r="H60" s="73"/>
-      <c r="I60" s="73"/>
-      <c r="J60" s="73"/>
-      <c r="K60" s="73"/>
-      <c r="L60" s="73"/>
-      <c r="M60" s="73"/>
-      <c r="N60" s="73"/>
-      <c r="O60" s="73"/>
-      <c r="P60" s="73"/>
-      <c r="Q60" s="73"/>
-      <c r="R60" s="73"/>
-      <c r="S60" s="73"/>
-      <c r="T60" s="73"/>
-      <c r="U60" s="73"/>
-      <c r="V60" s="73"/>
-      <c r="W60" s="73"/>
-      <c r="X60" s="73"/>
-      <c r="Y60" s="73"/>
-      <c r="Z60" s="73"/>
-      <c r="AA60" s="73"/>
-      <c r="AB60" s="73"/>
-      <c r="AC60" s="73"/>
-      <c r="AD60" s="73"/>
-      <c r="AE60" s="74"/>
+      <c r="E60" s="83"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="83"/>
+      <c r="H60" s="83"/>
+      <c r="I60" s="83"/>
+      <c r="J60" s="83"/>
+      <c r="K60" s="83"/>
+      <c r="L60" s="83"/>
+      <c r="M60" s="83"/>
+      <c r="N60" s="83"/>
+      <c r="O60" s="83"/>
+      <c r="P60" s="83"/>
+      <c r="Q60" s="83"/>
+      <c r="R60" s="83"/>
+      <c r="S60" s="83"/>
+      <c r="T60" s="83"/>
+      <c r="U60" s="83"/>
+      <c r="V60" s="83"/>
+      <c r="W60" s="83"/>
+      <c r="X60" s="83"/>
+      <c r="Y60" s="83"/>
+      <c r="Z60" s="83"/>
+      <c r="AA60" s="83"/>
+      <c r="AB60" s="83"/>
+      <c r="AC60" s="83"/>
+      <c r="AD60" s="83"/>
+      <c r="AE60" s="84"/>
     </row>
     <row r="62" spans="2:31">
       <c r="C62" s="3" t="s">
@@ -5296,37 +8409,37 @@
       <c r="AE76" s="12"/>
     </row>
     <row r="77" spans="3:31" ht="27" customHeight="1">
-      <c r="C77" s="75" t="s">
+      <c r="C77" s="85" t="s">
         <v>239</v>
       </c>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="75"/>
-      <c r="J77" s="75"/>
-      <c r="K77" s="75"/>
-      <c r="L77" s="75"/>
-      <c r="M77" s="75"/>
-      <c r="N77" s="75"/>
-      <c r="O77" s="75"/>
-      <c r="P77" s="75"/>
-      <c r="Q77" s="75"/>
-      <c r="R77" s="75"/>
-      <c r="S77" s="75"/>
-      <c r="T77" s="75"/>
-      <c r="U77" s="75"/>
-      <c r="V77" s="75"/>
-      <c r="W77" s="75"/>
-      <c r="X77" s="75"/>
-      <c r="Y77" s="75"/>
-      <c r="Z77" s="75"/>
-      <c r="AA77" s="75"/>
-      <c r="AB77" s="75"/>
-      <c r="AC77" s="75"/>
-      <c r="AD77" s="75"/>
-      <c r="AE77" s="75"/>
+      <c r="D77" s="85"/>
+      <c r="E77" s="85"/>
+      <c r="F77" s="85"/>
+      <c r="G77" s="85"/>
+      <c r="H77" s="85"/>
+      <c r="I77" s="85"/>
+      <c r="J77" s="85"/>
+      <c r="K77" s="85"/>
+      <c r="L77" s="85"/>
+      <c r="M77" s="85"/>
+      <c r="N77" s="85"/>
+      <c r="O77" s="85"/>
+      <c r="P77" s="85"/>
+      <c r="Q77" s="85"/>
+      <c r="R77" s="85"/>
+      <c r="S77" s="85"/>
+      <c r="T77" s="85"/>
+      <c r="U77" s="85"/>
+      <c r="V77" s="85"/>
+      <c r="W77" s="85"/>
+      <c r="X77" s="85"/>
+      <c r="Y77" s="85"/>
+      <c r="Z77" s="85"/>
+      <c r="AA77" s="85"/>
+      <c r="AB77" s="85"/>
+      <c r="AC77" s="85"/>
+      <c r="AD77" s="85"/>
+      <c r="AE77" s="85"/>
     </row>
     <row r="78" spans="3:31">
       <c r="C78" t="s">
@@ -5602,36 +8715,36 @@
     </row>
     <row r="88" spans="2:31" ht="27.75" customHeight="1">
       <c r="C88" s="29"/>
-      <c r="D88" s="72" t="s">
+      <c r="D88" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="E88" s="73"/>
-      <c r="F88" s="73"/>
-      <c r="G88" s="73"/>
-      <c r="H88" s="73"/>
-      <c r="I88" s="73"/>
-      <c r="J88" s="73"/>
-      <c r="K88" s="73"/>
-      <c r="L88" s="73"/>
-      <c r="M88" s="73"/>
-      <c r="N88" s="73"/>
-      <c r="O88" s="73"/>
-      <c r="P88" s="73"/>
-      <c r="Q88" s="73"/>
-      <c r="R88" s="73"/>
-      <c r="S88" s="73"/>
-      <c r="T88" s="73"/>
-      <c r="U88" s="73"/>
-      <c r="V88" s="73"/>
-      <c r="W88" s="73"/>
-      <c r="X88" s="73"/>
-      <c r="Y88" s="73"/>
-      <c r="Z88" s="73"/>
-      <c r="AA88" s="73"/>
-      <c r="AB88" s="73"/>
-      <c r="AC88" s="73"/>
-      <c r="AD88" s="73"/>
-      <c r="AE88" s="74"/>
+      <c r="E88" s="83"/>
+      <c r="F88" s="83"/>
+      <c r="G88" s="83"/>
+      <c r="H88" s="83"/>
+      <c r="I88" s="83"/>
+      <c r="J88" s="83"/>
+      <c r="K88" s="83"/>
+      <c r="L88" s="83"/>
+      <c r="M88" s="83"/>
+      <c r="N88" s="83"/>
+      <c r="O88" s="83"/>
+      <c r="P88" s="83"/>
+      <c r="Q88" s="83"/>
+      <c r="R88" s="83"/>
+      <c r="S88" s="83"/>
+      <c r="T88" s="83"/>
+      <c r="U88" s="83"/>
+      <c r="V88" s="83"/>
+      <c r="W88" s="83"/>
+      <c r="X88" s="83"/>
+      <c r="Y88" s="83"/>
+      <c r="Z88" s="83"/>
+      <c r="AA88" s="83"/>
+      <c r="AB88" s="83"/>
+      <c r="AC88" s="83"/>
+      <c r="AD88" s="83"/>
+      <c r="AE88" s="84"/>
     </row>
     <row r="89" spans="2:31">
       <c r="C89" s="29"/>
@@ -6782,32 +9895,32 @@
     </row>
     <row r="8" spans="2:26" ht="41.25" customHeight="1">
       <c r="B8" s="10"/>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="86" t="s">
         <v>249</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="76"/>
-      <c r="W8" s="76"/>
-      <c r="X8" s="76"/>
-      <c r="Y8" s="76"/>
-      <c r="Z8" s="77"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="86"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
+      <c r="X8" s="86"/>
+      <c r="Y8" s="86"/>
+      <c r="Z8" s="87"/>
     </row>
     <row r="9" spans="2:26">
       <c r="B9" s="10"/>
@@ -6969,7 +10082,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:Y123"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ19" sqref="AJ19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="12.75"/>
   <sheetData>
@@ -10515,29 +13630,29 @@
       </c>
     </row>
     <row r="30" spans="2:22" ht="33" customHeight="1">
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="89" t="s">
         <v>268</v>
       </c>
-      <c r="C30" s="79"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="79"/>
-      <c r="O30" s="79"/>
-      <c r="P30" s="79"/>
-      <c r="Q30" s="79"/>
-      <c r="R30" s="79"/>
-      <c r="S30" s="79"/>
-      <c r="T30" s="79"/>
-      <c r="U30" s="79"/>
-      <c r="V30" s="79"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="89"/>
+      <c r="N30" s="89"/>
+      <c r="O30" s="89"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="89"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="89"/>
+      <c r="T30" s="89"/>
+      <c r="U30" s="89"/>
+      <c r="V30" s="89"/>
     </row>
     <row r="31" spans="2:22">
       <c r="B31" s="49" t="s">
@@ -10555,28 +13670,28 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="91.5" customHeight="1">
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="88" t="s">
         <v>279</v>
       </c>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="78"/>
-      <c r="L35" s="78"/>
-      <c r="M35" s="78"/>
-      <c r="N35" s="78"/>
-      <c r="O35" s="78"/>
-      <c r="P35" s="78"/>
-      <c r="Q35" s="78"/>
-      <c r="R35" s="78"/>
-      <c r="S35" s="78"/>
-      <c r="T35" s="78"/>
-      <c r="U35" s="78"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="88"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="88"/>
+      <c r="N35" s="88"/>
+      <c r="O35" s="88"/>
+      <c r="P35" s="88"/>
+      <c r="Q35" s="88"/>
+      <c r="R35" s="88"/>
+      <c r="S35" s="88"/>
+      <c r="T35" s="88"/>
+      <c r="U35" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10590,4 +13705,395 @@
     <oddFooter>&amp;L&amp;"Symbol,Regular"Ó&amp;"Arial,Regular" Thach N. Le&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH373"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" style="47"/>
+    <col min="2" max="2" width="3.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="3.28515625" style="47"/>
+    <col min="8" max="16384" width="3.28515625" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="67">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="67"/>
+      <c r="B2" s="47" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="67"/>
+      <c r="C3" s="68" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="47" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="47" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" s="47" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34">
+      <c r="AH34" s="64" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34">
+      <c r="A35" s="67">
+        <v>2</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34">
+      <c r="B36" s="47" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34">
+      <c r="C37" s="47" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" ht="16.5" thickBot="1">
+      <c r="B39" s="69" t="s">
+        <v>307</v>
+      </c>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="66"/>
+    </row>
+    <row r="40" spans="1:34" ht="16.5" thickTop="1"/>
+    <row r="41" spans="1:34">
+      <c r="C41" s="47" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34">
+      <c r="B42" s="70">
+        <v>1</v>
+      </c>
+      <c r="C42" s="71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34">
+      <c r="C43" s="47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" s="70">
+        <v>2</v>
+      </c>
+      <c r="C69" s="71" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="99" spans="2:29">
+      <c r="C99" s="47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="2:29">
+      <c r="D100" s="47" t="s">
+        <v>314</v>
+      </c>
+      <c r="AC100" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="103" spans="2:29">
+      <c r="B103" s="70">
+        <v>3</v>
+      </c>
+      <c r="C103" s="71" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="104" spans="2:29">
+      <c r="B104" s="72"/>
+      <c r="C104" s="47" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="105" spans="2:29">
+      <c r="B105" s="72"/>
+    </row>
+    <row r="137" spans="2:3">
+      <c r="B137" s="70">
+        <v>4</v>
+      </c>
+      <c r="C137" s="71" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3">
+      <c r="B138" s="72"/>
+      <c r="C138" s="47" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3">
+      <c r="C139" s="47" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3">
+      <c r="C140" s="47" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3">
+      <c r="C141" s="47" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3">
+      <c r="B171" s="70">
+        <v>5</v>
+      </c>
+      <c r="C171" s="71" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3">
+      <c r="B205" s="70">
+        <v>6</v>
+      </c>
+      <c r="C205" s="71" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3">
+      <c r="C232" s="47" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3">
+      <c r="C238" s="47" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="239" spans="2:3">
+      <c r="B239" s="70">
+        <v>7</v>
+      </c>
+      <c r="C239" s="71" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="240" spans="2:3">
+      <c r="C240" s="47" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="273" spans="2:3">
+      <c r="B273" s="70">
+        <v>8</v>
+      </c>
+      <c r="C273" s="71" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="274" spans="2:3">
+      <c r="C274" s="47" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="307" spans="2:4">
+      <c r="B307" s="70">
+        <v>9</v>
+      </c>
+      <c r="C307" s="71" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="308" spans="2:4">
+      <c r="B308" s="70"/>
+      <c r="C308" s="47" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="309" spans="2:4">
+      <c r="D309" s="47" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="338" spans="2:3">
+      <c r="C338" s="47" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="341" spans="2:3">
+      <c r="B341" s="70">
+        <v>10</v>
+      </c>
+      <c r="C341" s="71" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="342" spans="2:3">
+      <c r="C342" s="47" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="372" spans="3:3">
+      <c r="C372" s="47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="373" spans="3:3">
+      <c r="C373" s="47" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AC100" location="Sakai!B94" display="2.c) Create &quot;Academic term&quot;"/>
+  </hyperlinks>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Symbol,Regular"Ó &amp;"Arial,Regular"Thach N. Le&amp;R&amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G239"/>
+  <sheetViews>
+    <sheetView topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="7" width="3.28515625" style="47"/>
+    <col min="8" max="16384" width="3.28515625" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="67">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="67"/>
+      <c r="B2" s="70">
+        <v>1</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="63"/>
+      <c r="C3" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="63"/>
+      <c r="C4" s="47" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="63"/>
+      <c r="C35" s="47" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="47" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="47" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3">
+      <c r="C103" s="47" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3">
+      <c r="B137" s="70">
+        <v>2</v>
+      </c>
+      <c r="C137" s="47" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3">
+      <c r="C171" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3">
+      <c r="C172" s="47" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="201" spans="3:3">
+      <c r="C201" s="47" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="205" spans="3:3">
+      <c r="C205" s="47" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="239" spans="3:3">
+      <c r="C239" s="47" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Symbol,Regular"Ó &amp;"Arial,Regular"Thach N. Le&amp;R&amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add guidelines to add users into the course site
</commit_message>
<xml_diff>
--- a/deploy-sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
+++ b/deploy-sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="11340" windowHeight="8535" tabRatio="991"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="11340" windowHeight="8535" tabRatio="991" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,9 @@
     <sheet name="MySQL" sheetId="5" r:id="rId7"/>
     <sheet name="Exercise01_CreateCourseSite" sheetId="50" r:id="rId8"/>
     <sheet name="Exercise02_CreateQuestionBank" sheetId="52" r:id="rId9"/>
-    <sheet name="Template" sheetId="53" state="hidden" r:id="rId10"/>
+    <sheet name="Exercise03_CreateAccount" sheetId="54" r:id="rId10"/>
+    <sheet name="Exercise04_CreateTestSession" sheetId="55" r:id="rId11"/>
+    <sheet name="Template" sheetId="53" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Linux!$A$1:$AE$146</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="393">
   <si>
     <t>#</t>
   </si>
@@ -1176,6 +1178,114 @@
   </si>
   <si>
     <t>Exercise02_CreateQuestionBank</t>
+  </si>
+  <si>
+    <t>Create local account on Sakai</t>
+  </si>
+  <si>
+    <t>Login by account admin.</t>
+  </si>
+  <si>
+    <t>Go to site "My Workspace", click on left menu Users.</t>
+  </si>
+  <si>
+    <t>Then click on button "New User"</t>
+  </si>
+  <si>
+    <t>Input information for user. Then click on button "Save Details".</t>
+  </si>
+  <si>
+    <t>Create Test session</t>
+  </si>
+  <si>
+    <t>Within the course site such as "JavaFresher", click on left menu "Tests &amp; Quizzes".</t>
+  </si>
+  <si>
+    <t>Select "Create using markup text"</t>
+  </si>
+  <si>
+    <t>Select "Chose assessment type (optional): Timed Test</t>
+  </si>
+  <si>
+    <t>Click on button "Next"</t>
+  </si>
+  <si>
+    <t>Click on button "Create Assessment"</t>
+  </si>
+  <si>
+    <t>Click on Action "Edit" of the Assessment.</t>
+  </si>
+  <si>
+    <t>Click on link "Edit" of the Part 1</t>
+  </si>
+  <si>
+    <t>Select Question Pools, number question will be drawed.</t>
+  </si>
+  <si>
+    <t>Input Title for the part.</t>
+  </si>
+  <si>
+    <t>Input point(s) for each correct answer.</t>
+  </si>
+  <si>
+    <t>Then click button "Save".</t>
+  </si>
+  <si>
+    <t>Add more Part if you want. Then select questions from a question pool similar above guidelines.</t>
+  </si>
+  <si>
+    <t>Click on link "Settings".</t>
+  </si>
+  <si>
+    <t>Setting available time, due time and limit duration for the test session.</t>
+  </si>
+  <si>
+    <t>Setting Layout and Appearance for the test session</t>
+  </si>
+  <si>
+    <t>Then click on button "Save Settings and Publish"</t>
+  </si>
+  <si>
+    <t>Click on button "Publish"</t>
+  </si>
+  <si>
+    <t>Now, all students of the site "JavaFresher" can perform the test from the available.</t>
+  </si>
+  <si>
+    <t>Setting Feedback Delivery: Feedback on submission</t>
+  </si>
+  <si>
+    <t>Monitor the progress of the test session and view result.</t>
+  </si>
+  <si>
+    <t>Select action "Score" to view and export the test result.</t>
+  </si>
+  <si>
+    <t>Exercise03_CreateAccount</t>
+  </si>
+  <si>
+    <t>Exercise04_CreateTestSession</t>
+  </si>
+  <si>
+    <t>Add users to the course site</t>
+  </si>
+  <si>
+    <t>Input the username of the account</t>
+  </si>
+  <si>
+    <t>Select role for user in the course site</t>
+  </si>
+  <si>
+    <t>Then click on button "Continue".</t>
+  </si>
+  <si>
+    <t>Click on button "Continue".</t>
+  </si>
+  <si>
+    <t>Click on the button "Finish"</t>
+  </si>
+  <si>
+    <t>View the result of adding account the the course site.</t>
   </si>
 </sst>
 </file>
@@ -4468,6 +4578,3224 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>187613</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="19802475"/>
+          <a:ext cx="7855238" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="600075"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rounded Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="1200150"/>
+          <a:ext cx="1123950" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="2190750"/>
+          <a:ext cx="600075" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>52388</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1366838" y="1543050"/>
+          <a:ext cx="795337" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rounded Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1743075" y="2171700"/>
+          <a:ext cx="600075" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1666875" y="2305050"/>
+          <a:ext cx="76200" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103804</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="7200900"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="13601700"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rounded Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5467350" y="14201775"/>
+          <a:ext cx="971550" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rounded Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="895349" y="16297275"/>
+          <a:ext cx="752475" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rounded Rectangle 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4067174" y="15135225"/>
+          <a:ext cx="876301" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rounded Rectangle 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1704974" y="21450300"/>
+          <a:ext cx="2343151" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rounded Rectangle 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="24907875"/>
+          <a:ext cx="581026" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>187613</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="25803225"/>
+          <a:ext cx="7855238" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rounded Rectangle 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714499" y="27803475"/>
+          <a:ext cx="4676775" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rounded Rectangle 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="28917900"/>
+          <a:ext cx="581026" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>187612</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>107896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1029" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438149" y="32003999"/>
+          <a:ext cx="7855238" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rounded Rectangle 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="34556700"/>
+          <a:ext cx="581026" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>187613</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1030" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="38004750"/>
+          <a:ext cx="7855238" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>187613</xdr:colOff>
+      <xdr:row>266</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1031" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="47605950"/>
+          <a:ext cx="7855238" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="43681650"/>
+          <a:ext cx="447675" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Rounded Rectangle 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1752600" y="52320826"/>
+          <a:ext cx="6191250" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="1000125"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rounded Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5457825" y="1600200"/>
+          <a:ext cx="942976" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="3400425"/>
+          <a:ext cx="1114426" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rounded Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1924049" y="4133849"/>
+          <a:ext cx="2028826" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1100138" y="1952625"/>
+          <a:ext cx="4829175" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1100138" y="3762375"/>
+          <a:ext cx="1838324" cy="371474"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2051" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="7000875"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Rounded Rectangle 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2152649" y="12011025"/>
+          <a:ext cx="447676" cy="371476"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>103805</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438151" y="13801725"/>
+          <a:ext cx="7771429" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190498</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rounded Rectangle 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2162173" y="16821150"/>
+          <a:ext cx="971551" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2053" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="20602575"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152398</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rounded Rectangle 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1904998" y="24203025"/>
+          <a:ext cx="971551" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2054" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="27403425"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rounded Rectangle 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7705725" y="30394275"/>
+          <a:ext cx="342899" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2055" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="34604325"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rounded Rectangle 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1790700" y="35271075"/>
+          <a:ext cx="3133725" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rounded Rectangle 42"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914525" y="38671500"/>
+          <a:ext cx="3400425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Rounded Rectangle 43"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190876" y="39671625"/>
+          <a:ext cx="723900" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2056" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="41005125"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>217</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rounded Rectangle 45"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1676401" y="43538775"/>
+          <a:ext cx="723900" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>266</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2057" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="47805975"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rounded Rectangle 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2257426" y="50044351"/>
+          <a:ext cx="533399" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>301</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2058" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="54806850"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rounded Rectangle 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2009776" y="57692926"/>
+          <a:ext cx="5657849" cy="828674"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>334</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2059" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="61407675"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>312</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rounded Rectangle 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885951" y="62474476"/>
+          <a:ext cx="5657849" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>315</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Rounded Rectangle 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2571751" y="63074551"/>
+          <a:ext cx="2305049" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>327</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>329</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rounded Rectangle 54"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2581276" y="65589151"/>
+          <a:ext cx="2305049" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>342</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2060" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="68408550"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>349</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rounded Rectangle 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2533651" y="69942076"/>
+          <a:ext cx="5000624" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Rounded Rectangle 57"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2533651" y="71161276"/>
+          <a:ext cx="5000624" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>375</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>402</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2061" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="75009375"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>394</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>395</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Rounded Rectangle 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1609726" y="78847951"/>
+          <a:ext cx="1362074" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>410</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>437</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2062" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="82010250"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>422</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Rounded Rectangle 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2962276" y="84258151"/>
+          <a:ext cx="495299" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>444</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>96185</xdr:colOff>
+      <xdr:row>471</xdr:row>
+      <xdr:rowOff>107897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2063" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="88811100"/>
+          <a:ext cx="7763810" cy="5508572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>456</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>458</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Rounded Rectangle 64"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3943351" y="91392376"/>
+          <a:ext cx="2190749" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>461</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>463</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Rounded Rectangle 65"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1952626" y="92335351"/>
+          <a:ext cx="1104899" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>463</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>472</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Straight Arrow Connector 67"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1676400" y="92678250"/>
+          <a:ext cx="838200" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4755,8 +8083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="A13:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4853,6 +8181,24 @@
         <v>355</v>
       </c>
     </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="17">
+        <v>5</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="17">
+        <v>6</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="C16" s="17"/>
+    </row>
     <row r="18" spans="3:3">
       <c r="C18" s="62"/>
     </row>
@@ -4863,6 +8209,8 @@
     <hyperlink ref="B12" location="Sakai!A1" display="Sakai"/>
     <hyperlink ref="B13" location="Exercise01_CreateCourseSite!A1" display="Exercise01_CreateCourseSite"/>
     <hyperlink ref="B14" location="Exercise02_CreateQuestionBank!A1" display="Exercise02_CreateQuestionBank"/>
+    <hyperlink ref="B15" location="Exercise03_CreateAccount!A1" display="Exercise03_CreateAccount"/>
+    <hyperlink ref="B16" location="Exercise04_CreateTestSession!A1" display="Exercise04_CreateTestSession"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.4" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4873,6 +8221,229 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G239"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="7" width="3.28515625" style="47"/>
+    <col min="8" max="16384" width="3.28515625" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="67">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" s="47" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="C33" s="47" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="47" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="67">
+        <v>2</v>
+      </c>
+      <c r="B69" s="71" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="47" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="47" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3">
+      <c r="C166" s="47" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3">
+      <c r="B171" s="47" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" s="47" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2">
+      <c r="B239" s="47" t="s">
+        <v>392</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H473"/>
+  <sheetViews>
+    <sheetView topLeftCell="A456" workbookViewId="0">
+      <selection activeCell="AB481" sqref="AB481"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="7" width="3.28515625" style="47"/>
+    <col min="8" max="16384" width="3.28515625" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="67">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="67"/>
+      <c r="B2" s="47" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="47" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="47" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="47" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="47" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="47" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="47" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" s="47" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" s="47" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" s="47" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3">
+      <c r="C203" s="47" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3">
+      <c r="B205" s="47" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2">
+      <c r="B239" s="47" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2">
+      <c r="B273" s="47" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2">
+      <c r="B307" s="47" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="341" spans="2:2">
+      <c r="B341" s="47" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="375" spans="2:2">
+      <c r="B375" s="47" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="409" spans="2:2">
+      <c r="B409" s="47" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2">
+      <c r="B440" s="47" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
+      <c r="A443" s="67">
+        <v>2</v>
+      </c>
+      <c r="B443" s="47" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="473" spans="8:8">
+      <c r="H473" s="63" t="s">
+        <v>383</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -13711,9 +17282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH373"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>
   <cols>
@@ -13995,8 +17564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15.75"/>

</xml_diff>